<commit_message>
registration form and readme update
</commit_message>
<xml_diff>
--- a/project-board.xlsx
+++ b/project-board.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://libertymutual-my.sharepoint.com/personal/christopher_shade_libertymutual_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n0294037\Downloads\Capstone 1 (HTML, CSS Bootstrap)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{97B4ACB8-862A-4E9A-BE40-0A343CF98733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB6755B6-96AF-4062-B1D4-A5ADC7934B9E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04B156C-0EC0-4567-A8EF-F62CBF58E2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8E61734B-0BF6-4CD7-851F-D06CDA03FDCA}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Kylie's Advice" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -600,8 +599,8 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,7 +769,7 @@
       <c r="B21" t="s">
         <v>14</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>44</v>
       </c>
     </row>
@@ -778,7 +777,7 @@
       <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>44</v>
       </c>
     </row>
@@ -918,6 +917,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -958,6 +958,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -988,5 +989,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>